<commit_message>
Study 2 and 4
</commit_message>
<xml_diff>
--- a/Study 2/Shocks/EnergyPLAN/1.5 TECH - 2050.xlsx
+++ b/Study 2/Shocks/EnergyPLAN/1.5 TECH - 2050.xlsx
@@ -11000,7 +11000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11050,6 +11050,326 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Production of electricity by biomass and waste</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>0.02928176795580111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Production of electricity by coal</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Production of electricity by gas</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0.04392265193370166</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Production of electricity by hydro</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0.05524861878453039</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Production of electricity by nuclear</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0.1325966850828729</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Production of electricity by petroleum and other oil derivatives</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Production of electricity by solar photovoltaic</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0.1850828729281768</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Production of electricity by wind</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>EU27</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0.5538674033149171</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="70">
     <dataValidation sqref="A2" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">

</xml_diff>